<commit_message>
aggiunti file e codice per la media voti di item e user, collaborative_filtering.py adesso ha dentro adj_cosine_sim. Aggiornato nostro map
</commit_message>
<xml_diff>
--- a/test/riepilogo test map.xlsx
+++ b/test/riepilogo test map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>our map</t>
   </si>
@@ -35,24 +35,35 @@
     <t>algoritmo</t>
   </si>
   <si>
-    <t>cb cosine skr4</t>
-  </si>
-  <si>
     <t>cbf srk20sim srk10rank</t>
   </si>
   <si>
-    <t>item base filtering skr2sim skr6rank</t>
-  </si>
-  <si>
     <t>cbf srk8sim no den rank</t>
+  </si>
+  <si>
+    <t>cf_AdjCosine_skr6cosine_bias_noDenRanking_test</t>
+  </si>
+  <si>
+    <t>0.00247</t>
+  </si>
+  <si>
+    <t>0.00288</t>
+  </si>
+  <si>
+    <t>cf_cosine_skr6cosine_bias_noDenRanking_test.csv</t>
+  </si>
+  <si>
+    <t>0.00209</t>
+  </si>
+  <si>
+    <t>0.00240</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.000000000000000"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
@@ -72,10 +83,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -104,24 +115,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -405,71 +413,70 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.28515625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7">
-        <v>2.1499999999999998E-2</v>
-      </c>
-      <c r="C2" s="7">
-        <v>2.88461538462E-3</v>
-      </c>
-      <c r="D2" s="4"/>
+      <c r="B2" s="5">
+        <v>4.1399999999999996E-3</v>
+      </c>
+      <c r="C2" s="5">
+        <v>5.7692307692300002E-3</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="7">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C3" s="7">
-        <v>0</v>
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5">
+        <v>3.5799999999999998E-3</v>
+      </c>
+      <c r="C3" s="5">
+        <v>5.2884615384600001E-3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="8">
-        <v>4.1399999999999996E-3</v>
-      </c>
-      <c r="C4" s="8">
-        <v>5.7692307692300002E-3</v>
+      <c r="A4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="8">
-        <v>3.5799999999999998E-3</v>
-      </c>
-      <c r="C5" s="8">
-        <v>5.2884615384600001E-3</v>
+      <c r="A5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
varie prove our map
</commit_message>
<xml_diff>
--- a/test/riepilogo test map.xlsx
+++ b/test/riepilogo test map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>our map</t>
   </si>
@@ -92,13 +92,73 @@
     <t>cf_AdjCosine_skr0cosine_bias_noDenRanking_test.csv</t>
   </si>
   <si>
-    <t>OK SE SI VEDONO I DATI STESSI</t>
-  </si>
-  <si>
     <t>adjusted cosine da definizione cremo togliendo user avg negli altri casi si toglie item avg</t>
   </si>
   <si>
     <t>cf_AdjCosine_skr200cosine_bias_noDenRanking_test.csv</t>
+  </si>
+  <si>
+    <t>hybrid_cbf_cf_w0.13cf_w0.87cbf_test.csv</t>
+  </si>
+  <si>
+    <t>0.00465</t>
+  </si>
+  <si>
+    <t>hybrid_cbf_cfAdjCosine_w0.13cf_w0.87cbf_test.csv</t>
+  </si>
+  <si>
+    <t>in private 0,00510</t>
+  </si>
+  <si>
+    <t>cf_AdjCosine_skr6cosine_bias_noDenRanking_popularity_test.csv</t>
+  </si>
+  <si>
+    <t>OK SE SI VEDONO I DATI SONO GLI STESSI - valori denominatore altissimi(30-1000)</t>
+  </si>
+  <si>
+    <t>0.00021</t>
+  </si>
+  <si>
+    <t>0.00515</t>
+  </si>
+  <si>
+    <t>0.00528</t>
+  </si>
+  <si>
+    <t>0.00673</t>
+  </si>
+  <si>
+    <t>in private 0,00500</t>
+  </si>
+  <si>
+    <t>hybrid_cbf_cfAdjCosine_w0.11cf_w0.89cbf_test.csv</t>
+  </si>
+  <si>
+    <t>hybrid_cbf_cf_w0.11cf_w0.89cbf_test.csv</t>
+  </si>
+  <si>
+    <t>0.00482</t>
+  </si>
+  <si>
+    <t>0.00721</t>
+  </si>
+  <si>
+    <t>0.00625</t>
+  </si>
+  <si>
+    <t>hybrid_cbf_cfAdjCosine_w0.1cf_w0.9cbf_test.csv</t>
+  </si>
+  <si>
+    <t>hybrid_cbf_cf_w0.15cf_w0.85cbf_test.csv</t>
+  </si>
+  <si>
+    <t>0.00435</t>
+  </si>
+  <si>
+    <t>in private 0,00480</t>
+  </si>
+  <si>
+    <t>0.00576</t>
   </si>
 </sst>
 </file>
@@ -146,7 +206,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,6 +225,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -178,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -204,6 +270,7 @@
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -484,15 +551,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.140625" customWidth="1"/>
     <col min="2" max="3" width="18.28515625" style="5" customWidth="1"/>
     <col min="4" max="4" width="81.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
@@ -574,20 +641,20 @@
         <v>7</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>7</v>
+        <v>23</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>7</v>
@@ -595,7 +662,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>7</v>
@@ -603,47 +670,127 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>10</v>
+        <v>19</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C14" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>12</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="D15" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D15">
+  <sortState ref="A2:D22">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
varie prove di submission e test per la popularity
</commit_message>
<xml_diff>
--- a/test/riepilogo test map.xlsx
+++ b/test/riepilogo test map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
   <si>
     <t>our map</t>
   </si>
@@ -35,9 +35,6 @@
     <t>algoritmo</t>
   </si>
   <si>
-    <t>cbf srk20sim srk10rank</t>
-  </si>
-  <si>
     <t>cbf srk8sim no den rank</t>
   </si>
   <si>
@@ -164,16 +161,37 @@
     <t>0.00518</t>
   </si>
   <si>
-    <t>cf_AdjCosine_skr6cosine_bias_noDenRanking_popularity1000</t>
-  </si>
-  <si>
     <t>0.00128</t>
   </si>
   <si>
-    <t>cf_AdjCosine_skr6cosine_bias_noDenRanking_popularity2000</t>
-  </si>
-  <si>
     <t>0.00321</t>
+  </si>
+  <si>
+    <t>0.00173</t>
+  </si>
+  <si>
+    <t>cf_AdjCosine_skr6cosine_bias_noDenRanking_popularity1000_test.csv</t>
+  </si>
+  <si>
+    <t>cf_AdjCosine_skr6cosine_bias_noDenRanking_popularity1500_test.csv</t>
+  </si>
+  <si>
+    <t>cf_AdjCosine_skr6cosine_bias_noDenRanking_popularity2000_test.csv</t>
+  </si>
+  <si>
+    <t>cf_AdjCosine_skr6cosine_bias_noDenRanking_popularity500_test.csv</t>
+  </si>
+  <si>
+    <t>cbf srk20sim srk10rank+25:25A262:242:272:25</t>
+  </si>
+  <si>
+    <t>0.00336</t>
+  </si>
+  <si>
+    <t>0.00144</t>
+  </si>
+  <si>
+    <t>0.00096</t>
   </si>
 </sst>
 </file>
@@ -566,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +611,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="B2" s="5">
         <v>4.1399999999999996E-3</v>
@@ -604,7 +622,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="5">
         <v>3.5799999999999998E-3</v>
@@ -615,220 +633,245 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
         <v>46</v>
       </c>
-      <c r="B14" t="s">
-        <v>49</v>
+      <c r="C14" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
         <v>47</v>
       </c>
+      <c r="C15" s="5" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
         <v>5</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C18" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>34</v>
+        <v>9</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>25</v>
+      <c r="A20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" t="s">
-        <v>45</v>
+        <v>23</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>33</v>
+        <v>43</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D24">
-    <sortCondition ref="A2"/>
+  <sortState ref="A2:D26">
+    <sortCondition ref="A26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
aggiornamento file test/riepilogo test map.xlsx con nuovi dati ultima consegna
</commit_message>
<xml_diff>
--- a/test/riepilogo test map.xlsx
+++ b/test/riepilogo test map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Polimi\Recommender system\challenge project\git\clear-project\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Federica\Desktop\clear-project\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="60">
   <si>
     <t>our map</t>
   </si>
@@ -192,6 +192,18 @@
   </si>
   <si>
     <t>0.00096</t>
+  </si>
+  <si>
+    <t>hybrid_cbf_cfAdjCosine_w0.13cf_w0.87cbf_popularity1000</t>
+  </si>
+  <si>
+    <t>0.00548</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>in private ?</t>
   </si>
 </sst>
 </file>
@@ -584,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,6 +881,20 @@
         <v>37</v>
       </c>
     </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:D26">
     <sortCondition ref="A26"/>

</xml_diff>

<commit_message>
Aggiornamento test/riepilogo test map.xlsx
</commit_message>
<xml_diff>
--- a/test/riepilogo test map.xlsx
+++ b/test/riepilogo test map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
   <si>
     <t>our map</t>
   </si>
@@ -203,7 +203,25 @@
     <t>…</t>
   </si>
   <si>
-    <t>in private ?</t>
+    <t>hybrid_cbf_cfAdjCosine_w0.13cf_w0.87cbf_popularity500</t>
+  </si>
+  <si>
+    <t>0.00588</t>
+  </si>
+  <si>
+    <t>hybrid_cbf_cf_w0.13cf_w0.87cbf_popularity1000</t>
+  </si>
+  <si>
+    <t>0.00573</t>
+  </si>
+  <si>
+    <t>in private 0,00473</t>
+  </si>
+  <si>
+    <t>in private 0,00601</t>
+  </si>
+  <si>
+    <t>in private 0,00548</t>
   </si>
 </sst>
 </file>
@@ -596,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,7 +910,35 @@
         <v>58</v>
       </c>
       <c r="D27" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>59</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aggiornato test/riepilogo test map.xlsx
</commit_message>
<xml_diff>
--- a/test/riepilogo test map.xlsx
+++ b/test/riepilogo test map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Federica\Desktop\clear-project\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Polimi\Recommender system\challenge project\git\clear-project\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
   <si>
     <t>our map</t>
   </si>
@@ -222,6 +222,12 @@
   </si>
   <si>
     <t>in private 0,00548</t>
+  </si>
+  <si>
+    <t>hybrid_cbf_cf_w0.13cf_w0.87cbf_popularity1000_biasGiusti</t>
+  </si>
+  <si>
+    <t>0.00556</t>
   </si>
 </sst>
 </file>
@@ -614,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,6 +947,14 @@
         <v>65</v>
       </c>
     </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:D26">
     <sortCondition ref="A26"/>

</xml_diff>

<commit_message>
prova bias skr 5
</commit_message>
<xml_diff>
--- a/test/riepilogo test map.xlsx
+++ b/test/riepilogo test map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
   <si>
     <t>our map</t>
   </si>
@@ -228,6 +228,12 @@
   </si>
   <si>
     <t>0.00556</t>
+  </si>
+  <si>
+    <t>hybrid_cbf_cf_w0.13cf_w0.87cbf_popularity1000_biasGiustiSkr5</t>
+  </si>
+  <si>
+    <t>0.00555</t>
   </si>
 </sst>
 </file>
@@ -620,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,6 +961,14 @@
         <v>67</v>
       </c>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:D26">
     <sortCondition ref="A26"/>

</xml_diff>